<commit_message>
fix owner full name
</commit_message>
<xml_diff>
--- a/src/Erc.Households.PrintBills.Api/Templates/bill_gas.xlsx
+++ b/src/Erc.Households.PrintBills.Api/Templates/bill_gas.xlsx
@@ -858,6 +858,159 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -870,9 +1023,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -887,9 +1037,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -936,58 +1083,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1015,147 +1156,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1593,7 +1593,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,402 +1653,384 @@
       <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="e">
+      <c r="A4" s="14" t="e">
         <f>bill_gas_companyfullname</f>
         <v>#NAME?</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="83"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="87" t="e">
+      <c r="H4" s="20" t="e">
         <f>bill_gas_CompanyStateRegistryCode</f>
         <v>#NAME?</v>
       </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="89" t="e">
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22" t="e">
         <f>bill_gas_companyfullname</f>
         <v>#NAME?</v>
       </c>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="91"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
     </row>
     <row r="5" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="86"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="95" t="e">
+      <c r="H5" s="28" t="e">
         <f>bill_gas_BranchOfficeBankFullName</f>
         <v>#NAME?</v>
       </c>
-      <c r="I5" s="95"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="93"/>
-      <c r="N5" s="94"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="99" t="e">
+      <c r="B6" s="32" t="e">
         <f>bill_gas_CompanyAddress</f>
         <v>#NAME?</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="104" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="105"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="107" t="e">
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="41" t="e">
         <f>bill_gas_CompanyAddress</f>
         <v>#NAME?</v>
       </c>
-      <c r="L6" s="107"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="107"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="98"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="108" t="e">
+      <c r="A7" s="31"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="42" t="e">
         <f>bill_gas_BranchOfficeIban</f>
         <v>#NAME?</v>
       </c>
-      <c r="I7" s="109"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="107"/>
-      <c r="M7" s="107"/>
-      <c r="N7" s="107"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="76" t="e">
+      <c r="B8" s="58" t="e">
         <f>bill_gas_AccountingPointName</f>
         <v>#NAME?</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="78" t="e">
+      <c r="E8" s="60" t="e">
         <f>bill_gas_OwnerFullName</f>
         <v>#NAME?</v>
       </c>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="22" t="e">
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="12" t="e">
         <f>"О/р: "&amp;bill_gas_AccountingPointName</f>
         <v>#NAME?</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="e">
+      <c r="B9" s="70" t="e">
         <f>bill_gas_AccountingPointAddress</f>
         <v>#NAME?</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22" t="e">
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="12" t="e">
         <f>"ПІБ: "&amp;bill_gas_OwnerFullName</f>
         <v>#NAME?</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="111" t="e">
+      <c r="A10" s="45" t="e">
         <f>"Рахунок за спожитий природний газ за " &amp;bill_gas_PeriodShortDate</f>
         <v>#NAME?</v>
       </c>
-      <c r="B10" s="111"/>
-      <c r="C10" s="111"/>
-      <c r="D10" s="111"/>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="22" t="e">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="12" t="e">
         <f>bill_gas_AccountingPointAddress</f>
         <v>#NAME?</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="111"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="111"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="16" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="111"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="16" t="e">
+      <c r="A12" s="45"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="13" t="e">
         <f>"за "&amp;bill_gas_PeriodShortDate</f>
         <v>#NAME?</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="74"/>
       <c r="E13" s="6" t="e">
         <f>bill_gas_AccountingPointDebtHistory</f>
         <v>#NAME?</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="77"/>
       <c r="J13" s="7" t="e">
         <f>bill_gas_PaymentSumByPeriod</f>
         <v>#NAME?</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="33" t="e">
+      <c r="L13" s="79"/>
+      <c r="M13" s="82" t="e">
         <f>bill_gas_AccountingPointDebt</f>
         <v>#NAME?</v>
       </c>
-      <c r="N13" s="34"/>
+      <c r="N13" s="83"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="46" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="50" t="s">
+      <c r="G14" s="95"/>
+      <c r="H14" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="51"/>
-      <c r="J14" s="54" t="s">
+      <c r="I14" s="99"/>
+      <c r="J14" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="31"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="36"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="85"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="29" t="e">
+      <c r="A15" s="88"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="100"/>
+      <c r="K15" s="78" t="e">
         <f>bill_gas_CompanyShortName &amp;" Email: "&amp;bill_gas_CompanyEmail&amp; ", "&amp;bill_gas_CompanySite&amp;", тел." &amp;bill_gas_CompanyPhone</f>
         <v>#NAME?</v>
       </c>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="30"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="79"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="59" t="e">
+      <c r="A16" s="88"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="106" t="e">
         <f>bill_gas_TariffRate</f>
         <v>#NAME?</v>
       </c>
-      <c r="G16" s="60"/>
-      <c r="H16" s="65" t="e">
+      <c r="G16" s="107"/>
+      <c r="H16" s="46" t="e">
         <f>bill_gas_InvoiceTotalUnits</f>
         <v>#NAME?</v>
       </c>
-      <c r="I16" s="66"/>
-      <c r="J16" s="70" t="e">
+      <c r="I16" s="47"/>
+      <c r="J16" s="52" t="e">
         <f>bill_gas_InvoiceTotalAmountDue</f>
         <v>#NAME?</v>
       </c>
-      <c r="K16" s="56"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="58"/>
+      <c r="K16" s="103"/>
+      <c r="L16" s="104"/>
+      <c r="M16" s="104"/>
+      <c r="N16" s="105"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="12" t="s">
+      <c r="A17" s="88"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="A18" s="91"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="69"/>
       <c r="J19" s="8" t="e">
         <f>bill_gas_AccountingPointDebt</f>
         <v>#NAME?</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="A4:F5"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:N5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:G7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:N7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="A10:J12"/>
-    <mergeCell ref="H16:I18"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="E8:J8"/>
     <mergeCell ref="K17:N20"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="K12:N12"/>
@@ -2065,12 +2047,27 @@
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K15:N16"/>
     <mergeCell ref="F16:G18"/>
+    <mergeCell ref="H16:I18"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="A4:F5"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:N5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:G7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:N7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="A10:J12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="22" max="16383" man="1"/>
-  </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>